<commit_message>
added data in excell
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>employeeId</t>
   </si>
@@ -35,31 +35,25 @@
     <t>birthday</t>
   </si>
   <si>
-    <t>Shahzad Hussain</t>
-  </si>
-  <si>
-    <t>shahzada</t>
+    <t>Ram</t>
   </si>
   <si>
     <t>07-02-1992</t>
   </si>
   <si>
-    <t>Hussain</t>
-  </si>
-  <si>
-    <t>ejaz</t>
+    <t>Gaurav</t>
   </si>
   <si>
     <t>05-10-1994</t>
   </si>
   <si>
-    <t>sahil</t>
+    <t>Anuj</t>
   </si>
   <si>
     <t>19-07-2003</t>
   </si>
   <si>
-    <t>shahid</t>
+    <t>Monu</t>
   </si>
   <si>
     <t>11-02-1965</t>
@@ -78,6 +72,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -166,7 +161,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -202,16 +197,17 @@
         <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="b">
+      <c r="E2" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,19 +215,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,19 +236,20 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="b">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,19 +257,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="E5" s="1" t="b">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>